<commit_message>
Aggiornati data.json e report
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111080XXXXXXXX/Lepida/Lepida_CVPI/2.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111080XXXXXXXX/Lepida/Lepida_CVPI/2.0.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="320">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -762,13 +762,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-24T15:40:22Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03f7e95b6011a255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.604ab230e2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-05-29T22:57:36Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9a1dded8dfa83621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.df057dea9a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT2</t>
@@ -780,13 +780,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-24T15:40:23Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e4fc6c56a99bdb88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.dd5497d492^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-05-29T22:57:37Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7a660742e8950f86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.e7931acbfd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT3</t>
@@ -798,10 +798,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-24T15:40:24Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">affd202e7e2e7607</t>
+    <t xml:space="preserve">2024-05-29T22:57:39Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59bad8c567c63f19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.86b331356d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT4</t>
@@ -813,13 +816,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-24T15:40:25Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ffc1e92e0851f567</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.d5cda8dd24^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-05-29T22:57:40Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74b270ce8bc13489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.52481215d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT5_KO</t>
@@ -1087,13 +1090,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-24T15:40:21Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c3118ffb70536b8b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.6bd831c959^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-05-29T22:57:35Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3607f6cefb09204d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.d7e72b330b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">ID TEST CASE OK</t>
@@ -1766,10 +1769,10 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J42 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2840,10 +2843,10 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J42 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -3949,27 +3952,27 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E54" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J42" activeCellId="0" sqref="J42"/>
+      <selection pane="bottomLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+      <selection pane="bottomRight" activeCell="H56" activeCellId="0" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="38.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="38.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="18.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="59.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="104.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="25.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="26.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="33.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="11" width="36.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="11" width="27.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="11" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="11" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="11" width="36.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="11" width="31.86"/>
@@ -5529,7 +5532,7 @@
         <v>163</v>
       </c>
       <c r="F35" s="29" t="n">
-        <v>45436</v>
+        <v>45441</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>164</v>
@@ -5573,7 +5576,7 @@
         <v>168</v>
       </c>
       <c r="F36" s="29" t="n">
-        <v>45436</v>
+        <v>45441</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>169</v>
@@ -5617,7 +5620,7 @@
         <v>173</v>
       </c>
       <c r="F37" s="29" t="n">
-        <v>45436</v>
+        <v>45441</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>174</v>
@@ -5625,8 +5628,8 @@
       <c r="H37" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="I37" s="11" t="s">
-        <v>76</v>
+      <c r="I37" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="J37" s="32" t="s">
         <v>55</v>
@@ -5655,22 +5658,22 @@
         <v>71</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F38" s="29" t="n">
-        <v>45436</v>
+        <v>45441</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J38" s="32" t="s">
         <v>55</v>
@@ -5699,20 +5702,20 @@
         <v>71</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
       <c r="J39" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K39" s="32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L39" s="32"/>
       <c r="M39" s="32"/>
@@ -5737,19 +5740,19 @@
         <v>71</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F40" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I40" s="11" t="s">
         <v>76</v>
@@ -5791,20 +5794,20 @@
         <v>71</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F41" s="29"/>
       <c r="G41" s="29"/>
       <c r="H41" s="29"/>
       <c r="I41" s="29"/>
       <c r="J41" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K41" s="32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L41" s="32"/>
       <c r="M41" s="32"/>
@@ -5829,22 +5832,22 @@
         <v>71</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F42" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J42" s="32" t="s">
         <v>55</v>
@@ -5883,22 +5886,22 @@
         <v>71</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F43" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J43" s="32" t="s">
         <v>55</v>
@@ -5937,22 +5940,22 @@
         <v>71</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F44" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J44" s="32" t="s">
         <v>55</v>
@@ -5991,22 +5994,22 @@
         <v>71</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F45" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J45" s="32" t="s">
         <v>55</v>
@@ -6045,20 +6048,20 @@
         <v>71</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F46" s="29"/>
       <c r="G46" s="29"/>
       <c r="H46" s="29"/>
       <c r="I46" s="29"/>
       <c r="J46" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K46" s="32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L46" s="32"/>
       <c r="M46" s="32"/>
@@ -6083,22 +6086,22 @@
         <v>71</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F47" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J47" s="32" t="s">
         <v>55</v>
@@ -6137,20 +6140,20 @@
         <v>71</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F48" s="29"/>
       <c r="G48" s="29"/>
       <c r="H48" s="29"/>
       <c r="I48" s="29"/>
       <c r="J48" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K48" s="32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L48" s="32"/>
       <c r="M48" s="32"/>
@@ -6175,22 +6178,22 @@
         <v>71</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F49" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J49" s="32" t="s">
         <v>55</v>
@@ -6229,22 +6232,22 @@
         <v>71</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F50" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="J50" s="32" t="s">
         <v>55</v>
@@ -6283,22 +6286,22 @@
         <v>71</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F51" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J51" s="32" t="s">
         <v>55</v>
@@ -6337,22 +6340,22 @@
         <v>71</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F52" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J52" s="32" t="s">
         <v>55</v>
@@ -6391,22 +6394,22 @@
         <v>71</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F53" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J53" s="32" t="s">
         <v>55</v>
@@ -6445,22 +6448,22 @@
         <v>71</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F54" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J54" s="32" t="s">
         <v>55</v>
@@ -6499,20 +6502,20 @@
         <v>71</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F55" s="29"/>
       <c r="G55" s="29"/>
       <c r="H55" s="29"/>
       <c r="I55" s="29"/>
       <c r="J55" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K55" s="32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L55" s="32"/>
       <c r="M55" s="32"/>
@@ -6537,22 +6540,22 @@
         <v>49</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F56" s="29" t="n">
         <v>45436</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J56" s="32" t="s">
         <v>55</v>
@@ -6581,22 +6584,22 @@
         <v>71</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F57" s="29" t="n">
-        <v>45436</v>
+        <v>45441</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="J57" s="32" t="s">
         <v>55</v>
@@ -11638,13 +11641,13 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A9" activeCellId="1" sqref="J42 A9"/>
+      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="102"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.86"/>
@@ -11658,66 +11661,66 @@
         <v>29</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D5" s="38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11725,41 +11728,41 @@
         <v>49</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11767,83 +11770,83 @@
         <v>71</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C11" s="38" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C12" s="38" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C13" s="38" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C14" s="38" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11851,41 +11854,41 @@
         <v>49</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C15" s="38" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C16" s="38" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C17" s="38" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11893,69 +11896,69 @@
         <v>71</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C18" s="38" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C19" s="38" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C20" s="38" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C21" s="38" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C22" s="38" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11963,41 +11966,41 @@
         <v>49</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C23" s="38" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C24" s="38" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C25" s="38" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12005,69 +12008,69 @@
         <v>71</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C26" s="38" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C27" s="38" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C28" s="38" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C29" s="38" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C30" s="38" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12075,41 +12078,41 @@
         <v>49</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C31" s="38" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C32" s="38" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C33" s="38" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12117,21 +12120,21 @@
         <v>71</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C34" s="38" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C35" s="38" t="n">
         <v>195</v>
@@ -12142,10 +12145,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C36" s="38" t="n">
         <v>211</v>
@@ -12156,10 +12159,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C37" s="38" t="n">
         <v>227</v>
@@ -12170,10 +12173,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C38" s="38" t="n">
         <v>243</v>
@@ -12187,7 +12190,7 @@
         <v>49</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C39" s="38" t="n">
         <v>259</v>
@@ -12198,10 +12201,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C40" s="38" t="n">
         <v>275</v>
@@ -12212,10 +12215,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C41" s="38" t="n">
         <v>291</v>
@@ -12229,7 +12232,7 @@
         <v>71</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C42" s="38" t="n">
         <v>307</v>
@@ -12240,10 +12243,10 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C43" s="38" t="n">
         <v>196</v>
@@ -12254,10 +12257,10 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C44" s="38" t="n">
         <v>212</v>
@@ -12268,10 +12271,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C45" s="38" t="n">
         <v>228</v>
@@ -12282,10 +12285,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C46" s="38" t="n">
         <v>244</v>
@@ -12299,7 +12302,7 @@
         <v>49</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C47" s="38" t="n">
         <v>260</v>
@@ -12310,10 +12313,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C48" s="38" t="n">
         <v>276</v>
@@ -12324,10 +12327,10 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C49" s="38" t="n">
         <v>292</v>
@@ -12341,7 +12344,7 @@
         <v>71</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C50" s="38" t="n">
         <v>308</v>
@@ -13319,10 +13322,10 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J42 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -13339,7 +13342,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>55</v>
@@ -13347,10 +13350,10 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Aggiornati file con nuovi test
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111080XXXXXXXX/Lepida/Lepida_CVPI/2.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111080XXXXXXXX/Lepida/Lepida_CVPI/2.0.0/report-checklist.xlsx
@@ -762,13 +762,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-29T22:57:36Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9a1dded8dfa83621</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.df057dea9a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-05-30T21:14:53Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b54470f1fc7ee420</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.abae9b7d0d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT2</t>
@@ -780,13 +780,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-29T22:57:37Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7a660742e8950f86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.e7931acbfd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-05-30T21:14:55Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7888b0bff8ef0582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.5a5652314b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT3</t>
@@ -798,13 +798,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-29T22:57:39Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59bad8c567c63f19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.86b331356d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-05-30T21:14:56Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ea593aaf03d0b83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.d3b73e6c01^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT4</t>
@@ -816,13 +816,13 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2024-05-29T22:57:40Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74b270ce8bc13489</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.52481215d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2024-05-30T21:14:57Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5a32c4b18dcc1fd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.80.3.1.4.4.736173ee74d930e556d58b87162a2f32bc02383a123808d438ea8244bfa6a3b9.bbb7829e3e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_PSS_CT5_KO</t>
@@ -1772,7 +1772,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
@@ -2846,7 +2846,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -3952,11 +3952,11 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
-      <selection pane="bottomRight" activeCell="H56" activeCellId="0" sqref="H56"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="I38" activeCellId="0" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5515,7 +5515,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="114.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="26" t="n">
         <v>170</v>
       </c>
@@ -5532,7 +5532,7 @@
         <v>163</v>
       </c>
       <c r="F35" s="29" t="n">
-        <v>45441</v>
+        <v>45442</v>
       </c>
       <c r="G35" s="11" t="s">
         <v>164</v>
@@ -5576,7 +5576,7 @@
         <v>168</v>
       </c>
       <c r="F36" s="29" t="n">
-        <v>45441</v>
+        <v>45442</v>
       </c>
       <c r="G36" s="11" t="s">
         <v>169</v>
@@ -5620,7 +5620,7 @@
         <v>173</v>
       </c>
       <c r="F37" s="29" t="n">
-        <v>45441</v>
+        <v>45442</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>174</v>
@@ -5664,7 +5664,7 @@
         <v>178</v>
       </c>
       <c r="F38" s="29" t="n">
-        <v>45441</v>
+        <v>45442</v>
       </c>
       <c r="G38" s="11" t="s">
         <v>179</v>
@@ -11644,7 +11644,7 @@
       <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -13325,7 +13325,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>

</xml_diff>